<commit_message>
Leetcode Questions & String
</commit_message>
<xml_diff>
--- a/Questions.xlsx
+++ b/Questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876FFB04-69ED-4614-B2BF-FB9FDCE860F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6138BCA9-1FE0-49D3-861A-23F9CB0835F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Easy</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>sum+=n%10; product*=n%10</t>
+  </si>
+  <si>
+    <t>missing-number</t>
+  </si>
+  <si>
+    <t>Use Cycle Sort</t>
   </si>
 </sst>
 </file>
@@ -389,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,14 +453,23 @@
         <v>10</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="https://leetcode.com/problems/palindrome-number" xr:uid="{E27A10E6-7C0E-4BB3-A0C3-B091DEE8700C}"/>
     <hyperlink ref="A3" r:id="rId2" display="https://leetcode.com/problems/majority-element" xr:uid="{F5212C32-3835-409A-BB6F-01345955707A}"/>
     <hyperlink ref="A4" r:id="rId3" display="https://leetcode.com/problems/concatenation-of-array/" xr:uid="{1DF5FE91-33A4-46DB-8895-02B421EDA9D2}"/>
     <hyperlink ref="A6" r:id="rId4" display="https://leetcode.com/problems/subtract-the-product-and-sum-of-digits-of-an-integer" xr:uid="{DC516D10-ABAC-4A32-8723-467633F9B41F}"/>
+    <hyperlink ref="A7" r:id="rId5" display="https://leetcode.com/problems/missing-number" xr:uid="{5D9552C0-9E25-412A-83DD-EA16FA223D9B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>